<commit_message>
Overhaul README & example data
</commit_message>
<xml_diff>
--- a/data/example_gcms_results.xlsx
+++ b/data/example_gcms_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puter\Documents\codeprojects\fa_example_analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puter\Documents\codeprojects\example-fatty-acid-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661EEB53-646B-49B1-B875-66DE14DAA5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E816EBF-3D9F-4BBC-A2C4-4B6D6D315C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-3270" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>17:0 : Area</t>
   </si>
   <si>
-    <t>17:1w9c : Area</t>
-  </si>
-  <si>
     <t>18:0 : Area</t>
   </si>
   <si>
@@ -660,6 +657,9 @@
   </si>
   <si>
     <t>20:1w5</t>
+  </si>
+  <si>
+    <t>17:1w7c : Area</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF13" sqref="AF13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,96 +1579,96 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
+        <v>207</v>
+      </c>
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>40</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
       </c>
       <c r="E2">
         <v>53473</v>
@@ -1796,13 +1796,13 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
       </c>
       <c r="E3">
         <v>165690</v>
@@ -1930,13 +1930,13 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
       </c>
       <c r="E4">
         <v>332452</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
       </c>
       <c r="E5">
         <v>819567</v>
@@ -2198,13 +2198,13 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2334,13 +2334,13 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2606,13 +2606,13 @@
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2742,13 +2742,13 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2878,13 +2878,13 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3014,13 +3014,13 @@
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3150,13 +3150,13 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3286,13 +3286,13 @@
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -3422,13 +3422,13 @@
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3558,13 +3558,13 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3694,13 +3694,13 @@
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -3830,13 +3830,13 @@
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -3966,13 +3966,13 @@
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -4102,13 +4102,13 @@
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -4238,13 +4238,13 @@
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4374,13 +4374,13 @@
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -4510,13 +4510,13 @@
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -4646,13 +4646,13 @@
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4782,13 +4782,13 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -4918,13 +4918,13 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -5054,13 +5054,13 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -5190,13 +5190,13 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -5326,13 +5326,13 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -5462,13 +5462,13 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -5598,13 +5598,13 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31">
         <v>3065.5540105935575</v>
@@ -5734,13 +5734,13 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32">
         <v>866.57649610553767</v>
@@ -5870,13 +5870,13 @@
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33">
         <v>2755.9601668025439</v>
@@ -6006,13 +6006,13 @@
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34">
         <v>1654.0532017732955</v>
@@ -6142,13 +6142,13 @@
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35">
         <v>2471.5116966718356</v>
@@ -6278,13 +6278,13 @@
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36">
         <v>7357.307684317746</v>
@@ -6414,13 +6414,13 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -6550,13 +6550,13 @@
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38">
         <v>5593.6565976967167</v>
@@ -6686,13 +6686,13 @@
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39">
         <v>6001.5484687306962</v>
@@ -6822,13 +6822,13 @@
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40">
         <v>920.12338388733656</v>
@@ -6958,13 +6958,13 @@
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E41">
         <v>1596.5003243033971</v>
@@ -7094,13 +7094,13 @@
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42">
         <v>606.48333612432339</v>
@@ -7230,13 +7230,13 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E43">
         <v>606.96145653988663</v>
@@ -7366,13 +7366,13 @@
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E44">
         <v>5138.2449521442086</v>
@@ -7502,13 +7502,13 @@
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -7638,13 +7638,13 @@
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E46">
         <v>7830.6813130841811</v>
@@ -7774,13 +7774,13 @@
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47">
         <v>475.0508760632315</v>
@@ -7910,13 +7910,13 @@
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E48">
         <v>5806.5543658058568</v>
@@ -8046,13 +8046,13 @@
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E49">
         <v>8556.4274744692175</v>
@@ -8182,13 +8182,13 @@
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -8318,13 +8318,13 @@
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E51">
         <v>6315.137574743736</v>
@@ -8454,13 +8454,13 @@
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E52">
         <v>866.65840243037462</v>
@@ -8590,13 +8590,13 @@
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E53">
         <v>1420.9723605415002</v>
@@ -8726,13 +8726,13 @@
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E54">
         <v>5393.2611003703978</v>
@@ -8862,13 +8862,13 @@
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -8998,13 +8998,13 @@
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -9134,13 +9134,13 @@
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -9270,13 +9270,13 @@
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -9406,13 +9406,13 @@
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E59">
         <v>752.22906133850449</v>
@@ -9542,13 +9542,13 @@
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E60">
         <v>2929.8979419327534</v>
@@ -9678,13 +9678,13 @@
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E61">
         <v>827.41827568037922</v>
@@ -9814,13 +9814,13 @@
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E62">
         <v>2790.6316023760241</v>
@@ -9950,13 +9950,13 @@
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E63">
         <v>354.27568351742514</v>
@@ -10086,13 +10086,13 @@
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -10222,13 +10222,13 @@
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -10358,13 +10358,13 @@
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E66">
         <v>2382.1389784399762</v>
@@ -10494,13 +10494,13 @@
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E67">
         <v>2203.7212924020491</v>
@@ -10630,13 +10630,13 @@
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -10766,13 +10766,13 @@
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -10902,13 +10902,13 @@
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -11038,13 +11038,13 @@
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -11174,13 +11174,13 @@
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E72">
         <v>1301.3173439306388</v>
@@ -11310,13 +11310,13 @@
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -11446,13 +11446,13 @@
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -11582,13 +11582,13 @@
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E75">
         <v>2319.1311309085154</v>
@@ -11718,13 +11718,13 @@
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -11854,13 +11854,13 @@
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E77">
         <v>1619.0872274065068</v>
@@ -11990,13 +11990,13 @@
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -12126,13 +12126,13 @@
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -12262,13 +12262,13 @@
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E80">
         <v>0</v>

</xml_diff>